<commit_message>
Agregar Ejemplo PacienteCL y cambios varios
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-AuditEventCl.xlsx
+++ b/output/StructureDefinition-AuditEventCl.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.11</t>
+    <t>1.8.12</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-17T14:21:27-04:00</t>
+    <t>2024-06-21T18:30:18-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Cambio en el medication
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-AuditEventCl.xlsx
+++ b/output/StructureDefinition-AuditEventCl.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-27T08:59:20-04:00</t>
+    <t>2024-07-18T16:07:51-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -977,7 +977,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(PractitionerRole|Practitioner|Organization|Device|Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(https://hl7chile.cl/fhir/ig/clcore/StructureDefinition/CoreRolClinicoCl|https://hl7chile.cl/fhir/ig/clcore/StructureDefinition/CorePrestadorCl|https://hl7chile.cl/fhir/ig/clcore/StructureDefinition/CoreOrganizacionCl|https://hl7chile.cl/fhir/ig/clcore/StructureDefinition/CorePacienteCl|Device|RelatedPerson)
 </t>
   </si>
   <si>
@@ -1965,7 +1965,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="78.44140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>